<commit_message>
Save and load game working correctly just need to update side pins to also work when loading
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://galwaymayoinstitute-my.sharepoint.com/personal/g00389108_gmit_ie/Documents/2021_2022/App Development/Assignments/3- Mastermind/Mastermind/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{075A9B8D-C7F5-4CFD-95F8-FDF0DD3E84A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24649575-22C3-4983-9D7A-D326D67ADBCC}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{075A9B8D-C7F5-4CFD-95F8-FDF0DD3E84A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80AD9AE7-7F14-45D4-9FE2-FAAF8E41407F}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{962240CE-7041-49A1-A3C5-7DBBAB5784A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{962240CE-7041-49A1-A3C5-7DBBAB5784A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>Test</t>
   </si>
@@ -139,6 +139,21 @@
   </si>
   <si>
     <t>Load Game</t>
+  </si>
+  <si>
+    <t>When a user clicks save, data is saved to a file for a user to load later</t>
+  </si>
+  <si>
+    <t>when you click load, a saved game is loaded into the gameboard to continue</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>When a user clicks save the data is put into arrays however a file isnt created</t>
+  </si>
+  <si>
+    <t>as a file isnt created a past game cannot load to gameboard</t>
   </si>
 </sst>
 </file>
@@ -490,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC72F3EA-5261-4B02-A717-1978D60AACE2}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +517,7 @@
     <col min="2" max="2" width="2.88671875" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" customWidth="1"/>
     <col min="4" max="4" width="2.6640625" customWidth="1"/>
-    <col min="5" max="5" width="60.21875" customWidth="1"/>
+    <col min="5" max="5" width="65.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -672,10 +687,44 @@
       <c r="A20" t="s">
         <v>33</v>
       </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>